<commit_message>
chose one more paper
</commit_message>
<xml_diff>
--- a/literature/Final analysis.xlsx
+++ b/literature/Final analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="1540" windowWidth="30120" windowHeight="21400"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="2526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="2526">
   <si>
     <t>257?</t>
   </si>
@@ -7656,10 +7656,10 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -7733,7 +7733,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -7741,6 +7740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8024,8 +8024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F32" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="H38" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8757,7 +8757,7 @@
       <c r="G28" s="11" t="s">
         <v>1153</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="18" t="s">
         <v>1091</v>
       </c>
       <c r="I28" s="9"/>
@@ -9719,10 +9719,12 @@
       <c r="G65" s="11" t="s">
         <v>1085</v>
       </c>
-      <c r="H65" s="15" t="s">
+      <c r="H65" s="18" t="s">
         <v>1086</v>
       </c>
-      <c r="I65" s="9"/>
+      <c r="I65" s="9" t="s">
+        <v>2525</v>
+      </c>
       <c r="J65" s="9"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -18521,22 +18523,22 @@
       <c r="A410" s="2">
         <v>1</v>
       </c>
-      <c r="B410" s="18" t="s">
+      <c r="B410" s="17" t="s">
         <v>2511</v>
       </c>
-      <c r="C410" s="18" t="s">
+      <c r="C410" s="17" t="s">
         <v>2512</v>
       </c>
       <c r="D410" s="2">
         <v>2007</v>
       </c>
-      <c r="E410" s="18" t="s">
+      <c r="E410" s="17" t="s">
         <v>2513</v>
       </c>
-      <c r="F410" s="18" t="s">
+      <c r="F410" s="17" t="s">
         <v>2514</v>
       </c>
-      <c r="G410" s="18" t="s">
+      <c r="G410" s="17" t="s">
         <v>2515</v>
       </c>
       <c r="H410" s="13"/>
@@ -20153,7 +20155,7 @@
       <c r="A474" s="2">
         <v>0</v>
       </c>
-      <c r="B474" s="16" t="s">
+      <c r="B474" s="15" t="s">
         <v>1372</v>
       </c>
       <c r="C474" s="9" t="s">
@@ -20429,7 +20431,7 @@
       <c r="G484" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H484" s="17" t="s">
+      <c r="H484" s="16" t="s">
         <v>37</v>
       </c>
       <c r="I484" s="9"/>
@@ -21435,7 +21437,7 @@
       <c r="A524" s="2">
         <v>0</v>
       </c>
-      <c r="B524" s="16" t="s">
+      <c r="B524" s="15" t="s">
         <v>1252</v>
       </c>
       <c r="C524" s="9" t="s">
@@ -21969,7 +21971,7 @@
         <v>13</v>
       </c>
       <c r="I544" s="9"/>
-      <c r="J544" s="18" t="s">
+      <c r="J544" s="17" t="s">
         <v>2484</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reviewed one paper and added another
</commit_message>
<xml_diff>
--- a/literature/Final analysis.xlsx
+++ b/literature/Final analysis.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="2526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="2526">
   <si>
     <t>257?</t>
   </si>
@@ -8024,8 +8024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H38" workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" topLeftCell="H237" workbookViewId="0">
+      <selection activeCell="J251" sqref="J251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14460,7 +14460,9 @@
         <v>132</v>
       </c>
       <c r="H251" s="9"/>
-      <c r="I251" s="9"/>
+      <c r="I251" s="9" t="s">
+        <v>2525</v>
+      </c>
       <c r="J251" s="9" t="s">
         <v>2492</v>
       </c>
@@ -22048,7 +22050,7 @@
   </sheetData>
   <autoFilter ref="I1:I547"/>
   <sortState ref="A1:J547">
-    <sortCondition descending="1" ref="D174"/>
+    <sortCondition descending="1" ref="D1:D547"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="F549" r:id="rId1" display="https://doi.org/10.1016/j.jss.2016.09.043"/>

</xml_diff>

<commit_message>
added some more reading interests
</commit_message>
<xml_diff>
--- a/literature/Final analysis.xlsx
+++ b/literature/Final analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="28840" yWindow="1340" windowWidth="32380" windowHeight="21680"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="2526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="2527">
   <si>
     <t>257?</t>
   </si>
@@ -7611,6 +7611,9 @@
   </si>
   <si>
     <t>Levi</t>
+  </si>
+  <si>
+    <t>Sets the ground for learning, but no learning is done</t>
   </si>
 </sst>
 </file>
@@ -8024,8 +8027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H237" workbookViewId="0">
-      <selection activeCell="J251" sqref="J251"/>
+    <sheetView tabSelected="1" topLeftCell="F234" workbookViewId="0">
+      <selection activeCell="J265" sqref="J265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14030,7 +14033,9 @@
         <v>838</v>
       </c>
       <c r="H234" s="9"/>
-      <c r="I234" s="9"/>
+      <c r="I234" s="9" t="s">
+        <v>2525</v>
+      </c>
       <c r="J234" s="9"/>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.2">
@@ -14054,7 +14059,9 @@
       </c>
       <c r="G235" s="9"/>
       <c r="H235" s="9"/>
-      <c r="I235" s="9"/>
+      <c r="I235" s="9" t="s">
+        <v>2525</v>
+      </c>
       <c r="J235" s="9"/>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
@@ -14438,8 +14445,8 @@
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A251" s="2" t="s">
-        <v>8</v>
+      <c r="A251" s="2">
+        <v>1</v>
       </c>
       <c r="B251" s="9" t="s">
         <v>128</v>
@@ -14464,7 +14471,7 @@
         <v>2525</v>
       </c>
       <c r="J251" s="9" t="s">
-        <v>2492</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
selected paper for reading title Semantic Analysis of Functional and Non-Functional Requirements in Software Requirements Specifications
</commit_message>
<xml_diff>
--- a/literature/Final analysis.xlsx
+++ b/literature/Final analysis.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">final!$I$1:$I$551</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">final!$I$1:$I$551</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">final!$I$1:$I$551</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">final!$I$1:$I$551</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2749" uniqueCount="2540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="2540">
   <si>
     <t xml:space="preserve">257?</t>
   </si>
@@ -125,6 +126,9 @@
     <t xml:space="preserve">http://link.springer.com/chapter/10.1007/978-3-642-30353-1_42</t>
   </si>
   <si>
+    <t xml:space="preserve">Saad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Situation-Oriented Evaluation and Prioritization of Requirements</t>
   </si>
   <si>
@@ -2172,9 +2176,6 @@
   </si>
   <si>
     <t xml:space="preserve">10.1145/2593861.2593862</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saad</t>
   </si>
   <si>
     <t xml:space="preserve">Verifying Software Requirements Based on Answer Set Programming</t>
@@ -7948,23 +7949,19 @@
   </sheetPr>
   <dimension ref="A1:J551"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A132" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E154" activeCellId="0" sqref="E154"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.5459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="49.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="49.2704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8118,7 +8115,9 @@
         <v>31</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="J6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8126,20 +8125,20 @@
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -8150,20 +8149,20 @@
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -8174,25 +8173,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -8202,26 +8201,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J10" s="3"/>
     </row>
@@ -8230,20 +8229,20 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -8254,20 +8253,20 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -8278,20 +8277,20 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -8302,22 +8301,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J14" s="3"/>
     </row>
@@ -8326,26 +8325,26 @@
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J15" s="3"/>
     </row>
@@ -8354,26 +8353,26 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J16" s="3"/>
     </row>
@@ -8382,28 +8381,28 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -8412,22 +8411,22 @@
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>23</v>
@@ -8440,22 +8439,22 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>23</v>
@@ -8468,26 +8467,26 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J20" s="3"/>
     </row>
@@ -8496,26 +8495,26 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J21" s="3"/>
     </row>
@@ -8524,26 +8523,26 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J22" s="3"/>
     </row>
@@ -8552,24 +8551,24 @@
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J23" s="3"/>
     </row>
@@ -8578,24 +8577,24 @@
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J24" s="3"/>
     </row>
@@ -8604,24 +8603,24 @@
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J25" s="3"/>
     </row>
@@ -8630,20 +8629,20 @@
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -8654,23 +8653,23 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -8680,26 +8679,26 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J28" s="3"/>
     </row>
@@ -8708,25 +8707,25 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -8736,25 +8735,25 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -8764,25 +8763,25 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -8792,25 +8791,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D32" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -8820,22 +8819,22 @@
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>23</v>
@@ -8848,24 +8847,24 @@
         <v>1</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D34" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J34" s="8"/>
     </row>
@@ -8874,25 +8873,25 @@
         <v>9</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D35" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -8902,20 +8901,20 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -8926,20 +8925,20 @@
         <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -8950,20 +8949,20 @@
         <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -8974,20 +8973,20 @@
         <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -8998,20 +8997,20 @@
         <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -9022,20 +9021,20 @@
         <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -9046,20 +9045,20 @@
         <v>0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -9070,20 +9069,20 @@
         <v>0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -9094,20 +9093,20 @@
         <v>0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -9118,22 +9117,22 @@
         <v>0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -9144,22 +9143,22 @@
         <v>0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D46" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -9170,22 +9169,22 @@
         <v>0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -9196,19 +9195,19 @@
         <v>0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D48" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -9220,20 +9219,20 @@
         <v>9</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D49" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -9244,22 +9243,22 @@
         <v>9</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D50" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -9270,19 +9269,19 @@
         <v>9</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -9294,20 +9293,20 @@
         <v>9</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -9318,20 +9317,20 @@
         <v>9</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -9342,22 +9341,22 @@
         <v>9</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -9368,22 +9367,22 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -9394,28 +9393,28 @@
         <v>9</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J56" s="3"/>
     </row>
@@ -9424,28 +9423,28 @@
         <v>1</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D57" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J57" s="3"/>
     </row>
@@ -9454,26 +9453,26 @@
         <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J58" s="3"/>
     </row>
@@ -9482,26 +9481,26 @@
         <v>1</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D59" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J59" s="3"/>
     </row>
@@ -9510,28 +9509,28 @@
         <v>1</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J60" s="3"/>
     </row>
@@ -9540,26 +9539,26 @@
         <v>1</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D61" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J61" s="3"/>
     </row>
@@ -9568,28 +9567,28 @@
         <v>1</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D62" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J62" s="3"/>
     </row>
@@ -9598,28 +9597,28 @@
         <v>1</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D63" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J63" s="3"/>
     </row>
@@ -9628,24 +9627,24 @@
         <v>1</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D64" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J64" s="3"/>
     </row>
@@ -9654,26 +9653,26 @@
         <v>1</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D65" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J65" s="3"/>
     </row>
@@ -9682,23 +9681,23 @@
         <v>1</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D66" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
@@ -9708,20 +9707,20 @@
         <v>1</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D67" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
@@ -9732,23 +9731,23 @@
         <v>1</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D68" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
@@ -9758,24 +9757,24 @@
         <v>1</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D69" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J69" s="3"/>
     </row>
@@ -9784,26 +9783,26 @@
         <v>1</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D70" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J70" s="3"/>
     </row>
@@ -9812,26 +9811,26 @@
         <v>1</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D71" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J71" s="3"/>
     </row>
@@ -9840,22 +9839,22 @@
         <v>0</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D72" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -9866,20 +9865,20 @@
         <v>0</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D73" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -9890,20 +9889,20 @@
         <v>0</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D74" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -9914,20 +9913,20 @@
         <v>0</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D75" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -9938,20 +9937,20 @@
         <v>0</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D76" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -9962,20 +9961,20 @@
         <v>0</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D77" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -9986,23 +9985,23 @@
         <v>0</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D78" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
@@ -10012,20 +10011,20 @@
         <v>0</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D79" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -10036,20 +10035,20 @@
         <v>0</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D80" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -10060,20 +10059,20 @@
         <v>0</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D81" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -10084,20 +10083,20 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D82" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -10108,20 +10107,20 @@
         <v>0</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D83" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -10132,20 +10131,20 @@
         <v>0</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D84" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -10156,20 +10155,20 @@
         <v>0</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D85" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -10180,22 +10179,22 @@
         <v>0</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D86" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -10206,20 +10205,20 @@
         <v>0</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D87" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -10230,25 +10229,25 @@
         <v>0</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D88" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
@@ -10258,22 +10257,22 @@
         <v>0</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D89" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -10284,22 +10283,22 @@
         <v>0</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D90" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -10310,22 +10309,22 @@
         <v>0</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D91" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -10336,22 +10335,22 @@
         <v>0</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D92" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -10362,20 +10361,20 @@
         <v>0</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D93" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="E93" s="5"/>
       <c r="F93" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -10386,17 +10385,17 @@
         <v>9</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D94" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -10408,22 +10407,22 @@
         <v>9</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D95" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -10434,22 +10433,22 @@
         <v>9</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D96" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -10460,22 +10459,22 @@
         <v>9</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D97" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -10486,22 +10485,22 @@
         <v>9</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D98" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -10512,22 +10511,22 @@
         <v>9</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D99" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
@@ -10538,22 +10537,22 @@
         <v>9</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D100" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -10564,28 +10563,28 @@
         <v>1</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D101" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J101" s="3"/>
     </row>
@@ -10594,22 +10593,22 @@
         <v>1</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D102" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -10620,22 +10619,22 @@
         <v>1</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D103" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -10646,24 +10645,24 @@
         <v>1</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D104" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J104" s="3"/>
     </row>
@@ -10672,23 +10671,23 @@
         <v>1</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D105" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E105" s="5"/>
       <c r="F105" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
@@ -10698,22 +10697,22 @@
         <v>1</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D106" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -10724,23 +10723,23 @@
         <v>1</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D107" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="3" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H107" s="9" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
@@ -10750,22 +10749,22 @@
         <v>1</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D108" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -10776,25 +10775,25 @@
         <v>1</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D109" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
@@ -10804,17 +10803,17 @@
         <v>1</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D110" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="3" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
@@ -10826,20 +10825,20 @@
         <v>0</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D111" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
@@ -10850,22 +10849,22 @@
         <v>0</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D112" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -10876,20 +10875,20 @@
         <v>0</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D113" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="3" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -10900,20 +10899,20 @@
         <v>0</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D114" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
@@ -10924,20 +10923,20 @@
         <v>0</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D115" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="3" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -10948,20 +10947,20 @@
         <v>0</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D116" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -10972,20 +10971,20 @@
         <v>0</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D117" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -10996,17 +10995,17 @@
         <v>0</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D118" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="3" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
@@ -11018,22 +11017,22 @@
         <v>0</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D119" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
@@ -11044,19 +11043,19 @@
         <v>0</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D120" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
@@ -11068,22 +11067,22 @@
         <v>0</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D121" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -11094,22 +11093,22 @@
         <v>0</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D122" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -11120,22 +11119,22 @@
         <v>0</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D123" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
@@ -11146,22 +11145,22 @@
         <v>0</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D124" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -11172,22 +11171,22 @@
         <v>0</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D125" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
@@ -11198,22 +11197,22 @@
         <v>0</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D126" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
@@ -11224,20 +11223,20 @@
         <v>0</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D127" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="3" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -11248,23 +11247,23 @@
         <v>0</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D128" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E128" s="5"/>
       <c r="F128" s="3" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
@@ -11274,22 +11273,22 @@
         <v>0</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D129" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
@@ -11300,20 +11299,20 @@
         <v>0</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
@@ -11324,22 +11323,22 @@
         <v>0</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D131" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
@@ -11350,22 +11349,22 @@
         <v>0</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D132" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
@@ -11376,25 +11375,25 @@
         <v>0</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D133" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
@@ -11404,19 +11403,19 @@
         <v>0</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D134" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
@@ -11428,17 +11427,17 @@
         <v>0</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D135" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="3" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
@@ -11450,20 +11449,20 @@
         <v>9</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D136" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="3" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -11474,22 +11473,22 @@
         <v>9</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D137" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
@@ -11500,25 +11499,25 @@
         <v>9</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D138" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -11528,17 +11527,17 @@
         <v>9</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D139" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="3" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
@@ -11550,26 +11549,26 @@
         <v>1</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D140" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J140" s="3"/>
     </row>
@@ -11578,25 +11577,25 @@
         <v>1</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D141" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
@@ -11606,28 +11605,28 @@
         <v>1</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D142" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J142" s="3"/>
     </row>
@@ -11636,20 +11635,20 @@
         <v>1</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D143" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E143" s="5"/>
       <c r="F143" s="3" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="H143" s="3" t="s">
         <v>23</v>
@@ -11662,23 +11661,23 @@
         <v>1</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D144" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E144" s="5"/>
       <c r="F144" s="3" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -11688,17 +11687,17 @@
         <v>1</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D145" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E145" s="5"/>
       <c r="F145" s="3" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
@@ -11710,25 +11709,25 @@
         <v>1</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D146" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
@@ -11738,25 +11737,25 @@
         <v>1</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D147" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
@@ -11766,25 +11765,25 @@
         <v>1</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D148" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
@@ -11794,25 +11793,25 @@
         <v>1</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D149" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
@@ -11822,23 +11821,23 @@
         <v>1</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D150" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E150" s="5"/>
       <c r="F150" s="3" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="G150" s="6" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -11848,22 +11847,22 @@
         <v>1</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D151" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="G151" s="6" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
@@ -11874,19 +11873,19 @@
         <v>1</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D152" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
@@ -11898,24 +11897,24 @@
         <v>0</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D153" s="5" t="n">
         <v>2014</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3" t="s">
-        <v>715</v>
+        <v>32</v>
       </c>
       <c r="J153" s="3"/>
     </row>
@@ -12783,7 +12782,7 @@
       </c>
       <c r="H187" s="3"/>
       <c r="I187" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J187" s="3"/>
     </row>
@@ -12811,7 +12810,7 @@
       </c>
       <c r="H188" s="3"/>
       <c r="I188" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J188" s="3"/>
     </row>
@@ -13083,7 +13082,7 @@
       </c>
       <c r="H198" s="3"/>
       <c r="I198" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J198" s="3"/>
     </row>
@@ -14023,7 +14022,7 @@
       </c>
       <c r="H235" s="3"/>
       <c r="I235" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J235" s="3"/>
     </row>
@@ -14049,7 +14048,7 @@
       <c r="G236" s="3"/>
       <c r="H236" s="3"/>
       <c r="I236" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J236" s="3"/>
     </row>
@@ -14457,7 +14456,7 @@
       </c>
       <c r="H252" s="3"/>
       <c r="I252" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J252" s="3" t="s">
         <v>1181</v>
@@ -15416,7 +15415,7 @@
         <v>1353</v>
       </c>
       <c r="H290" s="11" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I290" s="3"/>
       <c r="J290" s="3" t="s">
@@ -15630,7 +15629,7 @@
         <v>1387</v>
       </c>
       <c r="H298" s="11" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I298" s="3"/>
       <c r="J298" s="3"/>
@@ -15839,7 +15838,7 @@
       <c r="G306" s="3"/>
       <c r="H306" s="3"/>
       <c r="I306" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J306" s="3"/>
     </row>
@@ -15917,7 +15916,7 @@
       </c>
       <c r="H309" s="3"/>
       <c r="I309" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J309" s="3"/>
     </row>
@@ -15939,7 +15938,7 @@
       <c r="G310" s="3"/>
       <c r="H310" s="3"/>
       <c r="I310" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J310" s="3"/>
     </row>
@@ -16887,7 +16886,7 @@
         <v>1392</v>
       </c>
       <c r="I347" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J347" s="3"/>
     </row>
@@ -17767,7 +17766,7 @@
         <v>1763</v>
       </c>
       <c r="I381" s="3" t="s">
-        <v>715</v>
+        <v>32</v>
       </c>
       <c r="J381" s="3"/>
     </row>
@@ -17871,7 +17870,7 @@
         <v>1777</v>
       </c>
       <c r="I385" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J385" s="3"/>
     </row>
@@ -18633,7 +18632,7 @@
       <c r="G415" s="3"/>
       <c r="H415" s="3"/>
       <c r="I415" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J415" s="3"/>
     </row>
@@ -18661,7 +18660,7 @@
       </c>
       <c r="H416" s="3"/>
       <c r="I416" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J416" s="3"/>
     </row>
@@ -18687,7 +18686,7 @@
       </c>
       <c r="H417" s="3"/>
       <c r="I417" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J417" s="3"/>
     </row>
@@ -20533,7 +20532,7 @@
         <v>1763</v>
       </c>
       <c r="I489" s="3" t="s">
-        <v>715</v>
+        <v>32</v>
       </c>
       <c r="J489" s="3"/>
     </row>

</xml_diff>

<commit_message>
created the classification/external theme and added one paper
</commit_message>
<xml_diff>
--- a/literature/Final analysis.xlsx
+++ b/literature/Final analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22780" windowHeight="15120" tabRatio="993"/>
+    <workbookView xWindow="29340" yWindow="2820" windowWidth="25880" windowHeight="19600" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2751" uniqueCount="2540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="2540">
   <si>
     <t>257?</t>
   </si>
@@ -8142,8 +8142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="I148" sqref="I148"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9912,7 +9912,9 @@
         <v>322</v>
       </c>
       <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
+      <c r="I67" s="3" t="s">
+        <v>299</v>
+      </c>
       <c r="J67" s="3"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added paper to database
</commit_message>
<xml_diff>
--- a/literature/Final analysis.xlsx
+++ b/literature/Final analysis.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="2540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="2543">
   <si>
     <t>257?</t>
   </si>
@@ -7659,6 +7659,15 @@
   </si>
   <si>
     <t>10.1145/800127.804087</t>
+  </si>
+  <si>
+    <t>Supporting Requirements Engineers in Recognising Security Issues</t>
+  </si>
+  <si>
+    <t>Eric Knauss, Siv Houmb, Kurt Schneider, Shareeful Islam and Jan Jurjens</t>
+  </si>
+  <si>
+    <t>https://pdfs.semanticscholar.org/a5f9/6e478f53327418f90382118b2f8aa3abe687.pdf</t>
   </si>
 </sst>
 </file>
@@ -7751,7 +7760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7793,6 +7802,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8142,16 +8157,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J551"/>
+  <dimension ref="A1:J552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="N57" sqref="N57"/>
+    <sheetView tabSelected="1" topLeftCell="A500" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="H549" sqref="H549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="59.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
     <col min="8" max="8" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22333,6 +22348,28 @@
       <c r="H551" s="3"/>
       <c r="I551" s="3"/>
       <c r="J551" s="3"/>
+    </row>
+    <row r="552" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A552" s="12">
+        <v>1</v>
+      </c>
+      <c r="B552" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C552" s="22" t="s">
+        <v>2541</v>
+      </c>
+      <c r="D552" s="12">
+        <v>2011</v>
+      </c>
+      <c r="E552" s="21"/>
+      <c r="F552" s="21" t="s">
+        <v>2542</v>
+      </c>
+      <c r="G552" s="21"/>
+      <c r="I552" t="s">
+        <v>299</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="I1:I551"/>
@@ -22527,6 +22564,6 @@
     <hyperlink ref="G311" r:id="rId188"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>